<commit_message>
Common: Added some other values
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/liquids.xlsx
+++ b/upgrade/fixtures/liquids.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE74703-EC9A-4DA0-943C-F5629EF163F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BD2E28-234F-412B-BCD1-5737554A1E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2655" yWindow="8520" windowWidth="23955" windowHeight="13320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1710" yWindow="7710" windowWidth="23955" windowHeight="13320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>tab</t>
   </si>
@@ -107,6 +107,12 @@
   </si>
   <si>
     <t>VCT Cinnamon</t>
+  </si>
+  <si>
+    <t>pg</t>
+  </si>
+  <si>
+    <t>vg</t>
   </si>
 </sst>
 </file>
@@ -480,20 +486,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7847F66-32D3-4015-A1DD-E1168BFD1F23}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="3" width="54.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" customWidth="1"/>
+    <col min="5" max="5" width="44.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -501,95 +509,167 @@
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>30</v>
+      </c>
+      <c r="D5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>50</v>
+      </c>
+      <c r="D8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>30</v>
+      </c>
+      <c r="D9">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
       <c r="B10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>100</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>100</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
+      </c>
+      <c r="C12">
+        <v>100</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Common: Added booster stuff
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/liquids.xlsx
+++ b/upgrade/fixtures/liquids.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BD2E28-234F-412B-BCD1-5737554A1E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4E81A2-6C11-4C85-8752-1EC1DDE8EEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1710" yWindow="7710" windowWidth="23955" windowHeight="13320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1365" yWindow="7365" windowWidth="23955" windowHeight="13320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="1" r:id="rId1"/>
@@ -489,7 +489,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +498,7 @@
     <col min="2" max="2" width="30.28515625" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" customWidth="1"/>
-    <col min="5" max="5" width="44.42578125" customWidth="1"/>
+    <col min="5" max="5" width="43" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -674,5 +674,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Common: Added liquid volume
</commit_message>
<xml_diff>
--- a/upgrade/fixtures/liquids.xlsx
+++ b/upgrade/fixtures/liquids.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marek Hanzal\Projects\github.com\marek-hanzal\puff-smith\upgrade\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4E81A2-6C11-4C85-8752-1EC1DDE8EEBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD3152C-6F59-4F19-878C-46A04103282A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1365" yWindow="7365" windowWidth="23955" windowHeight="13320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2010" yWindow="7965" windowWidth="23955" windowHeight="13320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabs" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>tab</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>vg</t>
+  </si>
+  <si>
+    <t>volume</t>
   </si>
 </sst>
 </file>
@@ -486,10 +489,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7847F66-32D3-4015-A1DD-E1168BFD1F23}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,10 +501,11 @@
     <col min="2" max="2" width="30.28515625" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" customWidth="1"/>
-    <col min="5" max="5" width="43" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -509,16 +513,19 @@
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -526,13 +533,16 @@
         <v>11</v>
       </c>
       <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="D2">
         <v>100</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -540,13 +550,16 @@
         <v>9</v>
       </c>
       <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3">
         <v>100</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -554,13 +567,16 @@
         <v>12</v>
       </c>
       <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4">
         <v>100</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -568,13 +584,16 @@
         <v>14</v>
       </c>
       <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
         <v>30</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -582,13 +601,16 @@
         <v>15</v>
       </c>
       <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
         <v>30</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -596,13 +618,16 @@
         <v>16</v>
       </c>
       <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
         <v>30</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -610,13 +635,16 @@
         <v>18</v>
       </c>
       <c r="C8">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D8">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -624,13 +652,16 @@
         <v>20</v>
       </c>
       <c r="C9">
+        <v>20</v>
+      </c>
+      <c r="D9">
         <v>30</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -638,13 +669,16 @@
         <v>22</v>
       </c>
       <c r="C10">
+        <v>20</v>
+      </c>
+      <c r="D10">
         <v>100</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -652,13 +686,16 @@
         <v>23</v>
       </c>
       <c r="C11">
+        <v>20</v>
+      </c>
+      <c r="D11">
         <v>100</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -666,9 +703,12 @@
         <v>26</v>
       </c>
       <c r="C12">
+        <v>20</v>
+      </c>
+      <c r="D12">
         <v>100</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>0</v>
       </c>
     </row>

</xml_diff>